<commit_message>
added tool for plotting school enrollment based on neighborhood
</commit_message>
<xml_diff>
--- a/data/enrollmentdata/SPS-AttendanceAreas.xlsx
+++ b/data/enrollmentdata/SPS-AttendanceAreas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamabear/Documents/GA-DSI/Projects/seattle-kids/data/enrollmentdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D704B9-BFB0-F141-BF2C-8192847286AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DA3A8B-FDC4-1743-B3B8-F4535DADCB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="3000" windowWidth="26040" windowHeight="14440" xr2:uid="{92816DED-9974-674B-8AD7-6E2E88FA1132}"/>
+    <workbookView xWindow="7700" yWindow="900" windowWidth="26040" windowHeight="14440" xr2:uid="{92816DED-9974-674B-8AD7-6E2E88FA1132}"/>
   </bookViews>
   <sheets>
     <sheet name="elementary" sheetId="1" r:id="rId1"/>
@@ -170,9 +170,6 @@
     <t>Genesee Hill , Fairmount Park, Pathfinder</t>
   </si>
   <si>
-    <t>Hay, Coe</t>
-  </si>
-  <si>
     <t>Lowell, Madison-Miller</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>Denny Int'l</t>
   </si>
   <si>
-    <t>Concord Int'l</t>
-  </si>
-  <si>
     <t>Roxhill, Highland Park</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>Aki Kurose</t>
   </si>
   <si>
-    <t>Hay</t>
-  </si>
-  <si>
     <t>McClure</t>
   </si>
   <si>
@@ -248,9 +239,6 @@
     <t>Nathan Hale</t>
   </si>
   <si>
-    <t>Broadview-Thomson K-8, Northgate</t>
-  </si>
-  <si>
     <t>Robert Eagle Staff</t>
   </si>
   <si>
@@ -266,21 +254,12 @@
     <t>Aki Kurose, Mercer Int'l</t>
   </si>
   <si>
-    <t>Beacon Hill Int'l, Kimball</t>
-  </si>
-  <si>
     <t>Mercer Int'l</t>
   </si>
   <si>
     <t>Franklin, Rainier Beach</t>
   </si>
   <si>
-    <t>Gatzert, Leschi, Thurgood Marshall</t>
-  </si>
-  <si>
-    <t>Viewlands, Bagley</t>
-  </si>
-  <si>
     <t>Greenwood</t>
   </si>
   <si>
@@ -299,22 +278,43 @@
     <t>Chief Sealth Int'l</t>
   </si>
   <si>
-    <t>B. F. Day, Greenlake</t>
-  </si>
-  <si>
-    <t>Greenlake, Laurelhurst</t>
-  </si>
-  <si>
     <t>Ingraham Int'l</t>
   </si>
   <si>
     <t>Aki Kurose, Washington, Meany</t>
   </si>
   <si>
-    <t>Thurgood Marshall, John Muir, Beacon Hill Int'l, Kimball, Leschi</t>
-  </si>
-  <si>
-    <t>Dearborn Park Int'l, Van Asselt, MLK Jr., Wing Luke, Dunlap, Hawthorne</t>
+    <t>Viewlands, Daniel Bagley</t>
+  </si>
+  <si>
+    <t>Broadview-Thomson, Northgate</t>
+  </si>
+  <si>
+    <t>Thurgood Marshall, John Muir, Beacon Hill Intl, Kimball, Leschi</t>
+  </si>
+  <si>
+    <t>Beacon Hill Intl, Kimball</t>
+  </si>
+  <si>
+    <t>Concord Intl</t>
+  </si>
+  <si>
+    <t>Green Lake, Laurelhurst</t>
+  </si>
+  <si>
+    <t>John Hay, Coe</t>
+  </si>
+  <si>
+    <t>John Hay</t>
+  </si>
+  <si>
+    <t>B. F. Day, Green Lake</t>
+  </si>
+  <si>
+    <t>Bailey Gatzert, Leschi, Thurgood Marshall</t>
+  </si>
+  <si>
+    <t>Dearborn Park, Van Asselt, Martin Luther King Jr., Wing Luke, Dunlap, Hawthorne</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,13 +699,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -727,13 +727,13 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -741,10 +741,10 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -755,13 +755,13 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -772,10 +772,10 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
         <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,13 +783,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -800,10 +800,10 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -811,13 +811,13 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -825,13 +825,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -842,7 +842,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
         <v>40</v>
@@ -853,10 +853,10 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -867,13 +867,13 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -881,13 +881,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -895,13 +895,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -909,10 +909,10 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -923,13 +923,13 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -937,13 +937,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -951,13 +951,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -968,10 +968,10 @@
         <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -979,10 +979,10 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -993,10 +993,10 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -1010,10 +1010,10 @@
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1021,13 +1021,13 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1035,10 +1035,10 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -1049,10 +1049,10 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>40</v>
@@ -1063,10 +1063,10 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
         <v>40</v>
@@ -1077,10 +1077,10 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
         <v>40</v>
@@ -1105,13 +1105,13 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1184,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1195,7 +1195,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
still working on getting dashboard that combines enrollment and population data.  Callback errors keep cropping up.  Need to rethink how dataframe format and probably combine some dfs
</commit_message>
<xml_diff>
--- a/data/enrollmentdata/SPS-AttendanceAreas.xlsx
+++ b/data/enrollmentdata/SPS-AttendanceAreas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamabear/Documents/GA-DSI/Projects/seattle-kids/data/enrollmentdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DA3A8B-FDC4-1743-B3B8-F4535DADCB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9665C4DD-B1DD-2B4F-BADE-D129070E2CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="900" windowWidth="26040" windowHeight="14440" xr2:uid="{92816DED-9974-674B-8AD7-6E2E88FA1132}"/>
+    <workbookView xWindow="2760" yWindow="900" windowWidth="26040" windowHeight="14440" xr2:uid="{92816DED-9974-674B-8AD7-6E2E88FA1132}"/>
   </bookViews>
   <sheets>
     <sheet name="elementary" sheetId="1" r:id="rId1"/>
@@ -669,7 +669,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed the combined neighborhood population and school enrollment dashboard
</commit_message>
<xml_diff>
--- a/data/enrollmentdata/SPS-AttendanceAreas.xlsx
+++ b/data/enrollmentdata/SPS-AttendanceAreas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamabear/Documents/GA-DSI/Projects/seattle-kids/data/enrollmentdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9665C4DD-B1DD-2B4F-BADE-D129070E2CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAB01A3-9F0D-6643-AEA3-E2F2CC4AC6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="900" windowWidth="26040" windowHeight="14440" xr2:uid="{92816DED-9974-674B-8AD7-6E2E88FA1132}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="92">
   <si>
     <t>neighborhood</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Lowell</t>
   </si>
   <si>
-    <t>Genesee Hill , Fairmount Park, Pathfinder</t>
-  </si>
-  <si>
     <t>Lowell, Madison-Miller</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>Eckstein</t>
   </si>
   <si>
-    <t>Greenlake</t>
-  </si>
-  <si>
     <t>Eckstein, Hamilton Int'l</t>
   </si>
   <si>
@@ -290,9 +284,6 @@
     <t>Broadview-Thomson, Northgate</t>
   </si>
   <si>
-    <t>Thurgood Marshall, John Muir, Beacon Hill Intl, Kimball, Leschi</t>
-  </si>
-  <si>
     <t>Beacon Hill Intl, Kimball</t>
   </si>
   <si>
@@ -311,10 +302,16 @@
     <t>B. F. Day, Green Lake</t>
   </si>
   <si>
-    <t>Bailey Gatzert, Leschi, Thurgood Marshall</t>
-  </si>
-  <si>
     <t>Dearborn Park, Van Asselt, Martin Luther King Jr., Wing Luke, Dunlap, Hawthorne</t>
+  </si>
+  <si>
+    <t>Bailey Gatzert, Leschi, T. Marshall</t>
+  </si>
+  <si>
+    <t>T. Marshall, John Muir, Beacon Hill Intl, Kimball, Leschi</t>
+  </si>
+  <si>
+    <t>Genesee Hill, Fairmount Park, Pathfinder</t>
   </si>
 </sst>
 </file>
@@ -669,7 +666,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,13 +696,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -713,7 +710,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -727,13 +724,13 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -741,10 +738,10 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -755,13 +752,13 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -772,10 +769,10 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
         <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,13 +780,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
         <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -800,10 +797,10 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -811,13 +808,13 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -825,13 +822,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -842,7 +839,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
         <v>40</v>
@@ -853,10 +850,10 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -867,13 +864,13 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
         <v>74</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -881,13 +878,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
         <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -895,13 +892,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -909,10 +906,10 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
         <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -923,13 +920,13 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -937,13 +934,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -951,13 +948,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -965,13 +962,13 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
         <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -979,10 +976,10 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
         <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>54</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -993,10 +990,10 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -1010,10 +1007,10 @@
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1021,13 +1018,13 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1035,10 +1032,10 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -1049,10 +1046,10 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
         <v>40</v>
@@ -1063,10 +1060,10 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
         <v>40</v>
@@ -1077,10 +1074,10 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
         <v>40</v>
@@ -1091,7 +1088,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
@@ -1105,13 +1102,13 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1181,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1195,7 +1192,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>